<commit_message>
Deluvio: Menu partly done.
</commit_message>
<xml_diff>
--- a/Deluvio/Deluvio.xlsx
+++ b/Deluvio/Deluvio.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9114"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="13395" windowHeight="5130" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="13395" windowHeight="5130"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="deluvio" localSheetId="1">Sheet2!$A$1:$D$84</definedName>
   </definedNames>
-  <calcPr calcId="144315"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="116">
   <si>
     <t>Датчик уровня жидкости омывателя</t>
   </si>
@@ -373,13 +373,22 @@
   </si>
   <si>
     <t>XTAL1</t>
+  </si>
+  <si>
+    <t>Бачок</t>
+  </si>
+  <si>
+    <t>Шланг омывателя 5м</t>
+  </si>
+  <si>
+    <t>Итого</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,16 +406,30 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -423,17 +446,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,34 +502,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1F497D" mc:Ignorable=""/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="EEECE1" mc:Ignorable=""/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="4F81BD" mc:Ignorable=""/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0504D" mc:Ignorable=""/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="9BBB59" mc:Ignorable=""/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="8064A2" mc:Ignorable=""/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="4BACC6" mc:Ignorable=""/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="F79646" mc:Ignorable=""/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0000FF" mc:Ignorable=""/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="800080" mc:Ignorable=""/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -642,7 +683,7 @@
         <a:effectStyle>
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+              <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
             </a:outerShdw>
@@ -651,7 +692,7 @@
         <a:effectStyle>
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+              <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
@@ -660,7 +701,7 @@
         <a:effectStyle>
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+              <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
@@ -737,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,11 +811,11 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>63</v>
-      </c>
-      <c r="D2">
+        <v>67</v>
+      </c>
+      <c r="D2" s="2">
         <f>B2*C2</f>
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -785,11 +826,50 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>140</v>
-      </c>
-      <c r="D3">
+        <v>120</v>
+      </c>
+      <c r="D3" s="2">
         <f>B3*C3</f>
-        <v>140</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D5" si="0">B4*C4</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8">
+        <f>SUM(D2:D7)</f>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -802,7 +882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Deluvio: looks like release-candidate.
</commit_message>
<xml_diff>
--- a/Deluvio/Deluvio.xlsx
+++ b/Deluvio/Deluvio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="13395" windowHeight="5130"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="13395" windowHeight="5130" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="124">
   <si>
     <t>Датчик уровня жидкости омывателя</t>
   </si>
@@ -382,6 +382,30 @@
   </si>
   <si>
     <t>Итого</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>Aref</t>
+  </si>
+  <si>
+    <t>mV</t>
+  </si>
+  <si>
+    <t>U treshold</t>
+  </si>
+  <si>
+    <t>Rup</t>
+  </si>
+  <si>
+    <t>Rdown</t>
+  </si>
+  <si>
+    <t>kOhm</t>
+  </si>
+  <si>
+    <t>U in</t>
   </si>
 </sst>
 </file>
@@ -466,12 +490,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -780,7 +805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1579,12 +1604,89 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2">
+        <v>3300</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3">
+        <v>8000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5">
+        <v>330</v>
+      </c>
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6">
+        <f>B3*B5/(B4+B5)</f>
+        <v>1984.9624060150377</v>
+      </c>
+      <c r="C6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="3">
+        <f>1024*B6/B2</f>
+        <v>615.93984962406023</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>